<commit_message>
ADDED: RestTemplate , Microservice registry
</commit_message>
<xml_diff>
--- a/HiredCandidateData.xlsx
+++ b/HiredCandidateData.xlsx
@@ -16,81 +16,207 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>hiredCity</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>hiredLab</t>
+  </si>
+  <si>
+    <t>Shubham</t>
+  </si>
+  <si>
+    <t>Yash</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>attitudeRemark</t>
+  </si>
+  <si>
+    <t>communicationRemark</t>
+  </si>
+  <si>
+    <t>knowledgeRemark</t>
+  </si>
+  <si>
+    <t>aggregateRemark</t>
+  </si>
+  <si>
+    <t>onboardingStatus</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>creatorUser</t>
+  </si>
+  <si>
+    <t>joinDate</t>
+  </si>
+  <si>
+    <t>aggPer</t>
+  </si>
+  <si>
+    <t>currentPinCode</t>
+  </si>
+  <si>
+    <t>permanentPincode</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>mobileNumber</t>
+  </si>
+  <si>
+    <t>hiredDate</t>
+  </si>
+  <si>
+    <t>Sunil</t>
+  </si>
+  <si>
+    <t>Omkar</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Hemant</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Bandagale</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Mayekar</t>
+  </si>
+  <si>
+    <t>Avhad</t>
+  </si>
+  <si>
+    <t>Kamble</t>
+  </si>
+  <si>
+    <t>shuham@gmail.com</t>
+  </si>
+  <si>
+    <t>Bengal@gmail.com</t>
+  </si>
+  <si>
+    <t>Nagpur@gmail.com</t>
+  </si>
+  <si>
+    <t>Pune@gmail.com</t>
+  </si>
+  <si>
+    <t>Avhad@gmail.com</t>
+  </si>
+  <si>
+    <t>Kam@gmail.com</t>
+  </si>
+  <si>
+    <t>Nashik</t>
+  </si>
+  <si>
+    <t>Novemeber</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>B.E</t>
+  </si>
+  <si>
+    <t>Diploma</t>
+  </si>
+  <si>
+    <t>INFT</t>
+  </si>
+  <si>
+    <t>MECH</t>
+  </si>
+  <si>
+    <t>EXTC</t>
+  </si>
+  <si>
+    <t>ELEC</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t>Proper</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
   <si>
     <t>id</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>hiredCity</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>degree</t>
-  </si>
-  <si>
-    <t>hiredLab</t>
-  </si>
-  <si>
-    <t>Shubham</t>
-  </si>
-  <si>
-    <t>itsband97@gmail.com</t>
-  </si>
-  <si>
-    <t>Yash</t>
-  </si>
-  <si>
-    <t>Shardul</t>
-  </si>
-  <si>
-    <t>yash@gmail.com</t>
-  </si>
-  <si>
-    <t>shuarduL@gmail.com</t>
-  </si>
-  <si>
-    <t>Mumbai</t>
-  </si>
-  <si>
-    <t>BE</t>
-  </si>
-  <si>
-    <t>BBA</t>
-  </si>
-  <si>
-    <t>Com</t>
-  </si>
-  <si>
-    <t>It</t>
-  </si>
-  <si>
-    <t>Jharkhand</t>
-  </si>
-  <si>
-    <t>Bengal</t>
-  </si>
-  <si>
-    <t>Nagpur</t>
-  </si>
-  <si>
-    <t>Saurabh</t>
-  </si>
-  <si>
-    <t>borhade@gmial.com</t>
-  </si>
-  <si>
-    <t>Pune</t>
-  </si>
-  <si>
-    <t>Extc</t>
   </si>
 </sst>
 </file>
@@ -137,9 +263,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -435,137 +564,504 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
+      <c r="T1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:22">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2">
+        <v>9000460839</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2">
+        <v>60</v>
+      </c>
+      <c r="U2">
+        <v>400097</v>
+      </c>
+      <c r="V2">
+        <v>400097</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:22">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3">
+        <v>9004564566</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R3" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3">
+        <v>78</v>
+      </c>
+      <c r="U3">
+        <v>400097</v>
+      </c>
+      <c r="V3">
+        <v>400097</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:22">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>9000050000</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4" t="s">
+        <v>58</v>
+      </c>
+      <c r="P4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>61</v>
+      </c>
+      <c r="R4" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4">
+        <v>79</v>
+      </c>
+      <c r="U4">
+        <v>400097</v>
+      </c>
+      <c r="V4">
+        <v>400097</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:22">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5">
+        <v>8145098564</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5">
+        <v>5</v>
+      </c>
+      <c r="O5" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" t="s">
+        <v>65</v>
+      </c>
+      <c r="S5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5">
+        <v>67</v>
+      </c>
+      <c r="U5">
+        <v>400256</v>
+      </c>
+      <c r="V5">
+        <v>400256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6">
+        <v>8956485789</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6" t="s">
+        <v>58</v>
+      </c>
+      <c r="P6" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" t="s">
+        <v>65</v>
+      </c>
+      <c r="S6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T6">
+        <v>76</v>
+      </c>
+      <c r="U6">
+        <v>400235</v>
+      </c>
+      <c r="V6">
+        <v>400235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7">
+        <v>9004563632</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7" t="s">
+        <v>59</v>
+      </c>
+      <c r="P7" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>62</v>
+      </c>
+      <c r="R7" t="s">
+        <v>47</v>
+      </c>
+      <c r="S7" t="s">
+        <v>9</v>
+      </c>
+      <c r="T7">
+        <v>60</v>
+      </c>
+      <c r="U7">
+        <v>400009</v>
+      </c>
+      <c r="V7">
+        <v>400009</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>